<commit_message>
9 different test cases added ,6 test classes
</commit_message>
<xml_diff>
--- a/7rmartSupermarket/src/main/java/Resources/TestData.xlsx
+++ b/7rmartSupermarket/src/main/java/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreel\git\7rmartSupermarket\7rmartSupermarket\src\main\java\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C63AAF-2EBF-46D8-AF51-386CFEFB7A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC4A8B8-AE48-45F5-AD66-85F8B29D25FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -131,16 +131,16 @@
     <t>https://groceryapp.uniqassosiates.com/admin/list-offercode</t>
   </si>
   <si>
-    <t>ImageUrl</t>
-  </si>
-  <si>
     <t>Percentage</t>
   </si>
   <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>C:\Users\sreel\Desktop\JavaTraining\Selenium\code.png</t>
+    <t>https://groceryapp.uniqassosiates.com/admin/list-product</t>
+  </si>
+  <si>
+    <t>ManageProduct</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F79C24-1DC1-456E-A33D-61C4CBB06DA1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,10 +706,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
         <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -718,6 +718,7 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4A040EF3-BF1A-4A75-8563-C8699EE10B8E}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{834C5ABF-DF94-4EDD-A6BD-E7BA120563D0}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{016B499B-4584-4C09-A6D7-2A300EF1D182}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{17E7760A-2803-4786-A64C-A06085607E17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -727,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D645C4E4-9825-4BD1-BBB9-66B03E9AB1F6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -743,7 +744,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>177</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -815,10 +816,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>